<commit_message>
CREATEd preliminary VIEW, ssas.vw_Opportunnity, as fact for semantic layer; Added ClosedWonCt measure to Opportunity table;
</commit_message>
<xml_diff>
--- a/Requirements/Prototype.xlsx
+++ b/Requirements/Prototype.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,23 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phill\Source\Repos\ManBearPigSalesforcePipeline\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7910A31-C86E-4743-9795-2D75B4D44442}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E6EA75-3BE0-444F-AD23-9DF58252FB0B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9615"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="LeadsBySource" sheetId="1" r:id="rId1"/>
+    <sheet name="ClosedWon" sheetId="2" r:id="rId1"/>
+    <sheet name="LeadsBySource" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="19" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="52" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" odcFile="C:\Users\phill\AppData\Local\Temp\tmp98E7.odc" keepAlive="1" name="localhost:51050 SalesforceSM_phill_c7827562-917a-4e9c-8f3a-4b61f5b2a836" type="5" refreshedVersion="6" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{6D8F4577-03AC-4001-93AA-75C8F988BD99}" odcFile="C:\Users\phill\OneDrive\Documents\My Data Sources\desktop-td602cr_jabbotab SFAnalytics Model.odc" keepAlive="1" name="desktop-td602cr_jabbotab SFAnalytics Model" type="5" refreshedVersion="6" background="1">
+    <dbPr connection="Provider=MSOLAP.8;Integrated Security=SSPI;Persist Security Info=True;Initial Catalog=SFAnalytics;Data Source=desktop-td602cr\jabbotab;MDX Compatibility=1;Safety Options=2;MDX Missing Member Mode=Error;Update Isolation Level=2" command="Model" commandType="1"/>
+    <olapPr sendLocale="1" rowDrillCount="1000"/>
+  </connection>
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" odcFile="C:\Users\phill\AppData\Local\Temp\tmp98E7.odc" keepAlive="1" name="localhost:51050 SalesforceSM_phill_c7827562-917a-4e9c-8f3a-4b61f5b2a836" type="5" refreshedVersion="6" background="1">
     <dbPr connection="Provider=MSOLAP.8;Integrated Security=SSPI;Persist Security Info=True;Initial Catalog=SalesforceSM_phill_c7827562-917a-4e9c-8f3a-4b61f5b2a836;Data Source=localhost:51050;MDX Compatibility=1;Safety Options=2;MDX Missing Member Mode=Error;Optimize Response=3;Cell Error Mode=TextValue;Update Isolation Level=2" command="Model" commandType="1"/>
     <olapPr rowDrillCount="1000"/>
   </connection>
@@ -32,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>LeadCt</t>
   </si>
@@ -54,11 +60,68 @@
   <si>
     <t>Grand Total</t>
   </si>
+  <si>
+    <t>ClosedWonCt</t>
+  </si>
+  <si>
+    <t>7/28/2018</t>
+  </si>
+  <si>
+    <t>8/4/2018</t>
+  </si>
+  <si>
+    <t>8/7/2018</t>
+  </si>
+  <si>
+    <t>8/11/2018</t>
+  </si>
+  <si>
+    <t>8/15/2018</t>
+  </si>
+  <si>
+    <t>8/31/2018</t>
+  </si>
+  <si>
+    <t>9/1/2018</t>
+  </si>
+  <si>
+    <t>9/6/2018</t>
+  </si>
+  <si>
+    <t>9/14/2018</t>
+  </si>
+  <si>
+    <t>9/16/2018</t>
+  </si>
+  <si>
+    <t>9/18/2018</t>
+  </si>
+  <si>
+    <t>10/19/2018</t>
+  </si>
+  <si>
+    <t>10/22/2018</t>
+  </si>
+  <si>
+    <t>10/24/2018</t>
+  </si>
+  <si>
+    <t>11/2/2018</t>
+  </si>
+  <si>
+    <t>11/3/2018</t>
+  </si>
+  <si>
+    <t>11/7/2018</t>
+  </si>
+  <si>
+    <t>11/10/2018</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1672,8 +1735,8 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Phillip Raywood" refreshedDate="43419.675853935187" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
-  <cacheSource type="external" connectionId="1"/>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Phillip Raywood" refreshedDate="43419.675853935187" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF13000000}">
+  <cacheSource type="external" connectionId="2"/>
   <cacheFields count="2">
     <cacheField name="[Measures].[LeadCt]" caption="LeadCt" numFmtId="0" hierarchy="4" level="32767"/>
     <cacheField name="[Leads].[LeadSource].[LeadSource]" caption="LeadSource" numFmtId="0" hierarchy="3" level="1">
@@ -1721,8 +1784,212 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Phillip Raywood" refreshedDate="43420.325147685187" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{8FBF67BE-3727-43D5-BA8F-3342B40AEE94}">
+  <cacheSource type="external" connectionId="1"/>
+  <cacheFields count="2">
+    <cacheField name="[Measures].[ClosedWonCt]" caption="ClosedWonCt" numFmtId="0" hierarchy="13" level="32767"/>
+    <cacheField name="[Opportunity].[CloseDate].[CloseDate]" caption="CloseDate" numFmtId="0" hierarchy="4" level="1">
+      <sharedItems count="18">
+        <s v="[Opportunity].[CloseDate].&amp;[2018-07-28T00:00:00]" c="7/28/2018"/>
+        <s v="[Opportunity].[CloseDate].&amp;[2018-08-04T00:00:00]" c="8/4/2018"/>
+        <s v="[Opportunity].[CloseDate].&amp;[2018-08-07T00:00:00]" c="8/7/2018"/>
+        <s v="[Opportunity].[CloseDate].&amp;[2018-08-11T00:00:00]" c="8/11/2018"/>
+        <s v="[Opportunity].[CloseDate].&amp;[2018-08-15T00:00:00]" c="8/15/2018"/>
+        <s v="[Opportunity].[CloseDate].&amp;[2018-08-31T00:00:00]" c="8/31/2018"/>
+        <s v="[Opportunity].[CloseDate].&amp;[2018-09-01T00:00:00]" c="9/1/2018"/>
+        <s v="[Opportunity].[CloseDate].&amp;[2018-09-06T00:00:00]" c="9/6/2018"/>
+        <s v="[Opportunity].[CloseDate].&amp;[2018-09-14T00:00:00]" c="9/14/2018"/>
+        <s v="[Opportunity].[CloseDate].&amp;[2018-09-16T00:00:00]" c="9/16/2018"/>
+        <s v="[Opportunity].[CloseDate].&amp;[2018-09-18T00:00:00]" c="9/18/2018"/>
+        <s v="[Opportunity].[CloseDate].&amp;[2018-10-19T00:00:00]" c="10/19/2018"/>
+        <s v="[Opportunity].[CloseDate].&amp;[2018-10-22T00:00:00]" c="10/22/2018"/>
+        <s v="[Opportunity].[CloseDate].&amp;[2018-10-24T00:00:00]" c="10/24/2018"/>
+        <s v="[Opportunity].[CloseDate].&amp;[2018-11-02T00:00:00]" c="11/2/2018"/>
+        <s v="[Opportunity].[CloseDate].&amp;[2018-11-03T00:00:00]" c="11/3/2018"/>
+        <s v="[Opportunity].[CloseDate].&amp;[2018-11-07T00:00:00]" c="11/7/2018"/>
+        <s v="[Opportunity].[CloseDate].&amp;[2018-11-10T00:00:00]" c="11/10/2018"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <cacheHierarchies count="15">
+    <cacheHierarchy uniqueName="[Lead].[ConvertedDate]" caption="ConvertedDate" attribute="1" defaultMemberUniqueName="[Lead].[ConvertedDate].[All]" allUniqueName="[Lead].[ConvertedDate].[All]" dimensionUniqueName="[Lead]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Lead].[CreatedDate]" caption="CreatedDate" attribute="1" defaultMemberUniqueName="[Lead].[CreatedDate].[All]" allUniqueName="[Lead].[CreatedDate].[All]" dimensionUniqueName="[Lead]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Lead].[IsDeleted]" caption="IsDeleted" attribute="1" defaultMemberUniqueName="[Lead].[IsDeleted].[All]" allUniqueName="[Lead].[IsDeleted].[All]" dimensionUniqueName="[Lead]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Lead].[LeadSource]" caption="LeadSource" attribute="1" defaultMemberUniqueName="[Lead].[LeadSource].[All]" allUniqueName="[Lead].[LeadSource].[All]" dimensionUniqueName="[Lead]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Opportunity].[CloseDate]" caption="CloseDate" attribute="1" defaultMemberUniqueName="[Opportunity].[CloseDate].[All]" allUniqueName="[Opportunity].[CloseDate].[All]" dimensionUniqueName="[Opportunity]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Opportunity].[ConvertedDate]" caption="ConvertedDate" attribute="1" defaultMemberUniqueName="[Opportunity].[ConvertedDate].[All]" allUniqueName="[Opportunity].[ConvertedDate].[All]" dimensionUniqueName="[Opportunity]" displayFolder="" count="2" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Opportunity].[CreatedDate]" caption="CreatedDate" attribute="1" defaultMemberUniqueName="[Opportunity].[CreatedDate].[All]" allUniqueName="[Opportunity].[CreatedDate].[All]" dimensionUniqueName="[Opportunity]" displayFolder="" count="2" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Opportunity].[IsDeleted]" caption="IsDeleted" attribute="1" defaultMemberUniqueName="[Opportunity].[IsDeleted].[All]" allUniqueName="[Opportunity].[IsDeleted].[All]" dimensionUniqueName="[Opportunity]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Opportunity].[LastModifiedDate]" caption="LastModifiedDate" attribute="1" defaultMemberUniqueName="[Opportunity].[LastModifiedDate].[All]" allUniqueName="[Opportunity].[LastModifiedDate].[All]" dimensionUniqueName="[Opportunity]" displayFolder="" count="2" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Opportunity].[LastViewedDate]" caption="LastViewedDate" attribute="1" defaultMemberUniqueName="[Opportunity].[LastViewedDate].[All]" allUniqueName="[Opportunity].[LastViewedDate].[All]" dimensionUniqueName="[Opportunity]" displayFolder="" count="2" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Opportunity].[StageName]" caption="StageName" attribute="1" defaultMemberUniqueName="[Opportunity].[StageName].[All]" allUniqueName="[Opportunity].[StageName].[All]" dimensionUniqueName="[Opportunity]" displayFolder="" count="2" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Measures].[LeadCt]" caption="LeadCt" measure="1" displayFolder="" measureGroup="Lead" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[OpportunityCt]" caption="OpportunityCt" measure="1" displayFolder="" measureGroup="Opportunity" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[ClosedWonCt]" caption="ClosedWonCt" measure="1" displayFolder="" measureGroup="Opportunity" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[__Default measure]" caption="__Default measure" measure="1" displayFolder="" count="0" hidden="1"/>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <dimensions count="3">
+    <dimension name="Lead" uniqueName="[Lead]" caption="Lead"/>
+    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
+    <dimension name="Opportunity" uniqueName="[Opportunity]" caption="Opportunity"/>
+  </dimensions>
+  <measureGroups count="2">
+    <measureGroup name="Lead" caption="Lead"/>
+    <measureGroup name="Opportunity" caption="Opportunity"/>
+  </measureGroups>
+  <maps count="2">
+    <map measureGroup="0" dimension="0"/>
+    <map measureGroup="1" dimension="2"/>
+  </maps>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C41470A4-F001-46CE-A7FE-70F672B03002}" name="PivotTable3" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+  <location ref="A3:B22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
+      <items count="18">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="19">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField fld="0" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotHierarchies count="15">
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+  </pivotHierarchies>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <rowHierarchiesUsage count="1">
+    <rowHierarchyUsage hierarchyUsage="4"/>
+  </rowHierarchiesUsage>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
   <location ref="A1:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -2100,10 +2367,190 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F674FD66-0DD0-465D-87FE-2BA2FD95BEB7}">
+  <dimension ref="A3:B22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="1">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>